<commit_message>
Improved bootstrap Better design for cash deposit class. Add stub for holiday calendars.
</commit_message>
<xml_diff>
--- a/date2.xlsx
+++ b/date2.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -386,7 +386,7 @@
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="1">
         <f ca="1">TODAY() + INT(1000*RAND())</f>
-        <v>43779</v>
+        <v>43788</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -404,13 +404,13 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5">
         <f ca="1">DAY(B2)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6">
         <f ca="1">_xll.XLL.DATE(B3,B4,B5)</f>
-        <v>43778</v>
+        <v>43787</v>
       </c>
       <c r="C6" s="2">
         <f ca="1">B2-B6</f>
@@ -420,7 +420,7 @@
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7">
         <f ca="1">_xll.XLL.YYYYMMDD(B6)</f>
-        <v>20191110</v>
+        <v>20191119</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
@@ -438,7 +438,7 @@
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10">
         <f ca="1">MOD(B7,100)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>